<commit_message>
pr pa process O2
</commit_message>
<xml_diff>
--- a/GA_Report.xlsx
+++ b/GA_Report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="GA" sheetId="1" r:id="rId1"/>
+    <sheet name="Report" sheetId="1" r:id="rId1"/>
     <sheet name="Raw Data" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
@@ -376,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -386,16 +386,19 @@
         <v>Timestamp</v>
       </c>
       <c r="B1" t="str">
-        <v>Total Operation Hrs(Minute)</v>
+        <v>energyExport</v>
       </c>
       <c r="C1" t="str">
-        <v>OG Grid Operation Hrs(minute)</v>
+        <v>Grid Availability (%)</v>
       </c>
       <c r="D1" t="str">
-        <v>Grid Down(minute)</v>
+        <v>Plant Availability (%)</v>
       </c>
       <c r="E1" t="str">
-        <v>Grid Availability (%)</v>
+        <v>POA(kWh/m2)</v>
+      </c>
+      <c r="F1" t="str">
+        <v>PR (%)</v>
       </c>
     </row>
     <row r="2">
@@ -409,9 +412,12 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-0.04166666666666667</v>
       </c>
       <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>0</v>
       </c>
     </row>
@@ -426,183 +432,296 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>-0.04166666666666667</v>
       </c>
       <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>Actual Energy Export(kWh)</v>
+      </c>
+      <c r="B1" t="str">
+        <v>PQM Active Total Export(kWh)</v>
+      </c>
+      <c r="C1" t="str">
         <v>Timestamp</v>
       </c>
-      <c r="B1" t="str">
-        <v>MCR PQM</v>
-      </c>
-      <c r="C1" t="str">
-        <v>POA</v>
-      </c>
       <c r="D1" t="str">
-        <v>Grid Unavailibility</v>
+        <v>POA (w/m2)</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>2022-03-29 00:03</v>
+      <c r="A2">
+        <v>2000</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="C2" t="str">
+        <v>2022-03-29</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
-        <v>2022-03-29 01:03</v>
+      <c r="A3">
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="C3" t="str">
+        <v>2022-03-29</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="str">
-        <v>2022-03-29 01:03</v>
+      <c r="A4">
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2022-03-29</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="str">
-        <v>2022-03-29 01:03</v>
+      <c r="A5">
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2022-03-29</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="str">
-        <v>2022-03-29 00:03</v>
+      <c r="A6">
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2022-03-29</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="str">
-        <v>2022-04-30 05:04</v>
+      <c r="A7">
+        <v>2000</v>
       </c>
       <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2022-04-30</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="str">
-        <v>2022-04-30 06:04</v>
+      <c r="A8">
+        <v>0</v>
       </c>
       <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2022-04-30</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="str">
-        <v>2022-04-30 09:04</v>
+      <c r="A9">
+        <v>0</v>
       </c>
       <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2022-04-30</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="str">
-        <v>2022-04-30 06:04</v>
+      <c r="A10">
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
+        <v>2000</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2022-04-30</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="str">
-        <v>2022-04-30 10:04</v>
+      <c r="A11">
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
+        <v>2000</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2022-04-30</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>2000</v>
+      </c>
+      <c r="C12" t="str">
+        <v>2022-03-29 00:55:00</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>2000</v>
+      </c>
+      <c r="C13" t="str">
+        <v>2022-03-29 01:00:00</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>2000</v>
+      </c>
+      <c r="C14" t="str">
+        <v>2022-03-29 01:20:00</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>2000</v>
+      </c>
+      <c r="C15" t="str">
+        <v>2022-03-29 01:14:00</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>2000</v>
+      </c>
+      <c r="C16" t="str">
+        <v>2022-03-29 00:57:00</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>2000</v>
+      </c>
+      <c r="C17" t="str">
+        <v>2022-04-30 05:30:00</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>2000</v>
+      </c>
+      <c r="C18" t="str">
+        <v>2022-04-30 06:20:00</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>2000</v>
+      </c>
+      <c r="C19" t="str">
+        <v>2022-04-30 09:06:40</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>2000</v>
+      </c>
+      <c r="C20" t="str">
+        <v>2022-04-30 06:43:20</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>2000</v>
+      </c>
+      <c r="C21" t="str">
+        <v>2022-04-30 10:00:00</v>
+      </c>
+      <c r="D21">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>